<commit_message>
+ bổ sung lỗi
</commit_message>
<xml_diff>
--- a/Bao Cao Lien Tuc/DanhSachLoi.xlsx
+++ b/Bao Cao Lien Tuc/DanhSachLoi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>NHÓM: MONEY10
 MÔN: TMĐT
@@ -85,10 +85,7 @@
     <t>Quản lý giao dịch _ Nạp tiền</t>
   </si>
   <si>
-    <t>_ không lỗi và cũng không có thông báo đã nạp thành công chưa.</t>
-  </si>
-  <si>
-    <t>_ kiểm tra trong csdl với số thẻ đó nhưng tiền ko tăng -&gt; là sao ?</t>
+    <t>_ nhập số thẻ đúng (copy từ csdl tình trạng =1, =0 luôn) nhưng cứ báo tài khoản không đúng.</t>
   </si>
 </sst>
 </file>
@@ -188,14 +185,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,7 +498,7 @@
   <dimension ref="B3:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,13 +512,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -530,7 +527,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -565,7 +562,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>9</v>
@@ -574,7 +571,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -595,7 +592,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>3</v>
       </c>
@@ -611,16 +608,13 @@
     <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="4"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="F12" s="1"/>
     </row>

</xml_diff>